<commit_message>
correction on manual cliques cut and begging of oddholes cuts
</commit_message>
<xml_diff>
--- a/code/exemplo.xlsx
+++ b/code/exemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git-version\jssp\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\jssp\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5733A37C-96BE-49D8-8D51-2D59AC650E2D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD59B7B-5CD4-4DFD-93E8-AB7C03242AE5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{07FD2462-AA0A-43E4-858C-41630EA873DA}"/>
   </bookViews>
@@ -70,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -275,12 +281,40 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -589,13 +623,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA72EC1-36D7-4AFA-BD85-A1EE22D9C081}">
-  <dimension ref="A1:AP292"/>
+  <dimension ref="A1:AP361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="16770" ySplit="600" topLeftCell="AQ274" activePane="bottomLeft"/>
-      <selection activeCell="AP1" sqref="AP1"/>
+      <pane xSplit="16770" ySplit="600" topLeftCell="AQ219" activePane="bottomLeft"/>
       <selection pane="topRight" activeCell="AD1" sqref="AD1:AP1048576"/>
-      <selection pane="bottomLeft" activeCell="AE290" sqref="AE280:AK290"/>
+      <selection pane="bottomLeft" activeCell="G192" sqref="G192:N199"/>
       <selection pane="bottomRight" activeCell="AN210" sqref="AN210"/>
     </sheetView>
   </sheetViews>
@@ -2983,7 +3016,7 @@
       <c r="AA272" s="4"/>
       <c r="AB272" s="4"/>
     </row>
-    <row r="273" spans="11:35" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:42" x14ac:dyDescent="0.25">
       <c r="K273" s="4"/>
       <c r="L273" s="4"/>
       <c r="M273" s="4"/>
@@ -3003,7 +3036,7 @@
       <c r="AA273" s="4"/>
       <c r="AB273" s="4"/>
     </row>
-    <row r="274" spans="11:35" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:42" x14ac:dyDescent="0.25">
       <c r="P274" s="4"/>
       <c r="Q274" s="4"/>
       <c r="R274" s="4"/>
@@ -3016,130 +3049,1189 @@
       <c r="Y274" s="4"/>
       <c r="Z274" s="4"/>
     </row>
-    <row r="275" spans="11:35" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:42" x14ac:dyDescent="0.25">
       <c r="U275" s="1"/>
       <c r="V275" s="1"/>
       <c r="W275" s="1"/>
       <c r="X275" s="1"/>
     </row>
-    <row r="276" spans="11:35" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:42" x14ac:dyDescent="0.25">
       <c r="V276" s="1"/>
       <c r="W276" s="1"/>
       <c r="X276" s="1"/>
       <c r="Y276" s="1"/>
     </row>
-    <row r="277" spans="11:35" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:42" x14ac:dyDescent="0.25">
       <c r="W277" s="1"/>
       <c r="X277" s="1"/>
       <c r="Y277" s="1"/>
       <c r="Z277" s="1"/>
     </row>
-    <row r="280" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AC280" s="30"/>
-      <c r="AD280" s="2"/>
-      <c r="AE280" s="2"/>
-      <c r="AF280" s="2"/>
-      <c r="AG280" s="2"/>
-    </row>
-    <row r="281" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AD281" s="30"/>
-      <c r="AE281" s="2"/>
-      <c r="AF281" s="2"/>
-      <c r="AG281" s="2"/>
-      <c r="AH281" s="2"/>
-    </row>
-    <row r="282" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AE282" s="1"/>
-      <c r="AF282" s="1"/>
-      <c r="AG282" s="1"/>
-    </row>
-    <row r="283" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AE283" s="30"/>
-      <c r="AF283" s="2"/>
-      <c r="AG283" s="2"/>
-      <c r="AH283" s="2"/>
-      <c r="AI283" s="2"/>
-    </row>
-    <row r="284" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="Y284" s="3"/>
-      <c r="Z284" s="3"/>
-      <c r="AA284" s="3"/>
-      <c r="AB284" s="3"/>
-      <c r="AC284" s="3"/>
-      <c r="AD284" s="3"/>
-      <c r="AE284" s="3"/>
-    </row>
-    <row r="285" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="Z285" s="3"/>
-      <c r="AA285" s="3"/>
-      <c r="AB285" s="3"/>
-      <c r="AC285" s="3"/>
-      <c r="AD285" s="3"/>
-      <c r="AE285" s="3"/>
-      <c r="AF285" s="3"/>
-    </row>
-    <row r="286" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AA286" s="3"/>
-      <c r="AB286" s="3"/>
-      <c r="AC286" s="3"/>
-      <c r="AD286" s="3"/>
-      <c r="AE286" s="3"/>
-      <c r="AF286" s="3"/>
-      <c r="AG286" s="3"/>
-    </row>
-    <row r="287" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AB287" s="3"/>
-      <c r="AC287" s="3"/>
-      <c r="AD287" s="3"/>
-      <c r="AE287" s="3"/>
-      <c r="AF287" s="3"/>
-      <c r="AG287" s="3"/>
-      <c r="AH287" s="3"/>
-    </row>
-    <row r="288" spans="11:35" x14ac:dyDescent="0.25">
-      <c r="AC288" s="3"/>
-      <c r="AD288" s="3"/>
-      <c r="AE288" s="3"/>
-      <c r="AF288" s="3"/>
-      <c r="AG288" s="3"/>
-      <c r="AH288" s="3"/>
-      <c r="AI288" s="3"/>
-    </row>
-    <row r="289" spans="30:39" x14ac:dyDescent="0.25">
-      <c r="AD289" s="3"/>
-      <c r="AE289" s="3"/>
-      <c r="AF289" s="3"/>
-      <c r="AG289" s="3"/>
-      <c r="AH289" s="3"/>
-      <c r="AI289" s="3"/>
-      <c r="AJ289" s="3"/>
-    </row>
-    <row r="290" spans="30:39" x14ac:dyDescent="0.25">
-      <c r="AE290" s="3"/>
-      <c r="AF290" s="3"/>
-      <c r="AG290" s="3"/>
-      <c r="AH290" s="3"/>
-      <c r="AI290" s="3"/>
-      <c r="AJ290" s="3"/>
-      <c r="AK290" s="3"/>
-    </row>
-    <row r="291" spans="30:39" x14ac:dyDescent="0.25">
-      <c r="AF291" s="3"/>
-      <c r="AG291" s="3"/>
-      <c r="AH291" s="3"/>
-      <c r="AI291" s="3"/>
-      <c r="AJ291" s="3"/>
-      <c r="AK291" s="3"/>
-      <c r="AL291" s="3"/>
-    </row>
-    <row r="292" spans="30:39" x14ac:dyDescent="0.25">
-      <c r="AG292" s="3"/>
-      <c r="AH292" s="3"/>
-      <c r="AI292" s="3"/>
-      <c r="AJ292" s="3"/>
-      <c r="AK292" s="3"/>
-      <c r="AL292" s="3"/>
-      <c r="AM292" s="3"/>
+    <row r="279" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A279" s="32"/>
+      <c r="B279" s="32"/>
+      <c r="C279" s="32"/>
+      <c r="D279" s="32"/>
+      <c r="E279" s="32"/>
+      <c r="F279" s="32"/>
+      <c r="G279" s="32"/>
+      <c r="H279" s="32"/>
+      <c r="I279" s="32"/>
+      <c r="J279" s="32"/>
+      <c r="K279" s="32"/>
+      <c r="L279" s="32"/>
+      <c r="M279" s="32"/>
+      <c r="N279" s="32"/>
+      <c r="O279" s="32"/>
+      <c r="P279" s="32"/>
+      <c r="Q279" s="32"/>
+      <c r="R279" s="32"/>
+      <c r="S279" s="32"/>
+      <c r="T279" s="32"/>
+      <c r="U279" s="32"/>
+      <c r="V279" s="32"/>
+      <c r="W279" s="32"/>
+      <c r="X279" s="32"/>
+      <c r="Y279" s="32"/>
+      <c r="Z279" s="32"/>
+      <c r="AA279" s="32"/>
+      <c r="AB279" s="32"/>
+      <c r="AC279" s="32"/>
+      <c r="AD279" s="32"/>
+      <c r="AE279" s="32"/>
+      <c r="AF279" s="32"/>
+      <c r="AG279" s="32"/>
+      <c r="AH279" s="32"/>
+      <c r="AI279" s="32"/>
+      <c r="AJ279" s="32"/>
+      <c r="AK279" s="32"/>
+      <c r="AL279" s="32"/>
+      <c r="AM279" s="32"/>
+      <c r="AN279" s="32"/>
+      <c r="AO279" s="32"/>
+      <c r="AP279" s="32"/>
+    </row>
+    <row r="280" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="V280" s="4"/>
+      <c r="W280" s="4"/>
+      <c r="X280" s="4"/>
+      <c r="Y280" s="4"/>
+      <c r="Z280" s="4"/>
+      <c r="AA280" s="4"/>
+      <c r="AB280" s="4"/>
+      <c r="AC280" s="31"/>
+      <c r="AD280" s="4"/>
+      <c r="AE280" s="4"/>
+      <c r="AF280" s="4"/>
+      <c r="AG280" s="4"/>
+      <c r="AH280" s="4"/>
+      <c r="AI280" s="4"/>
+      <c r="AJ280" s="4"/>
+      <c r="AK280" s="4"/>
+      <c r="AL280" s="4"/>
+      <c r="AM280" s="4"/>
+    </row>
+    <row r="281" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F281" s="4"/>
+      <c r="G281" s="4"/>
+      <c r="H281" s="4"/>
+      <c r="I281" s="50"/>
+      <c r="J281" s="50"/>
+      <c r="K281" s="50"/>
+      <c r="L281" s="50"/>
+      <c r="M281" s="50"/>
+      <c r="N281" s="50"/>
+      <c r="O281" s="50"/>
+      <c r="P281" s="50"/>
+      <c r="Q281" s="50"/>
+      <c r="R281" s="50"/>
+      <c r="V281" s="4"/>
+      <c r="W281" s="4"/>
+      <c r="X281" s="4"/>
+      <c r="Y281" s="4"/>
+      <c r="Z281" s="4"/>
+      <c r="AA281" s="4"/>
+      <c r="AB281" s="4"/>
+      <c r="AC281" s="4"/>
+      <c r="AD281" s="31"/>
+      <c r="AE281" s="4"/>
+      <c r="AF281" s="4"/>
+      <c r="AG281" s="4"/>
+      <c r="AH281" s="4"/>
+      <c r="AI281" s="4"/>
+      <c r="AJ281" s="4"/>
+      <c r="AK281" s="4"/>
+      <c r="AL281" s="4"/>
+      <c r="AM281" s="4"/>
+    </row>
+    <row r="282" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F282" s="4"/>
+      <c r="G282" s="4"/>
+      <c r="H282" s="4"/>
+      <c r="I282" s="4"/>
+      <c r="J282" s="4"/>
+      <c r="K282" s="4"/>
+      <c r="L282" s="50"/>
+      <c r="M282" s="50"/>
+      <c r="N282" s="50"/>
+      <c r="O282" s="4"/>
+      <c r="P282" s="4"/>
+      <c r="V282" s="4"/>
+      <c r="W282" s="4"/>
+      <c r="X282" s="4"/>
+      <c r="Y282" s="4"/>
+      <c r="Z282" s="4"/>
+      <c r="AA282" s="4"/>
+      <c r="AB282" s="4"/>
+      <c r="AC282" s="4"/>
+      <c r="AD282" s="4"/>
+      <c r="AE282" s="4"/>
+      <c r="AF282" s="4"/>
+      <c r="AG282" s="4"/>
+      <c r="AH282" s="4"/>
+      <c r="AI282" s="4"/>
+      <c r="AJ282" s="4"/>
+      <c r="AK282" s="4"/>
+      <c r="AL282" s="4"/>
+      <c r="AM282" s="4"/>
+    </row>
+    <row r="283" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F283" s="4"/>
+      <c r="G283" s="4"/>
+      <c r="H283" s="4"/>
+      <c r="I283" s="4"/>
+      <c r="J283" s="4"/>
+      <c r="K283" s="50"/>
+      <c r="L283" s="50"/>
+      <c r="M283" s="50"/>
+      <c r="N283" s="50"/>
+      <c r="O283" s="50"/>
+      <c r="P283" s="50"/>
+      <c r="Q283" s="50"/>
+      <c r="R283" s="50"/>
+      <c r="V283" s="4"/>
+      <c r="W283" s="4"/>
+      <c r="X283" s="4"/>
+      <c r="Y283" s="4"/>
+      <c r="Z283" s="4"/>
+      <c r="AA283" s="4"/>
+      <c r="AB283" s="4"/>
+      <c r="AC283" s="4"/>
+      <c r="AD283" s="4"/>
+      <c r="AE283" s="31"/>
+      <c r="AF283" s="4"/>
+      <c r="AG283" s="4"/>
+      <c r="AH283" s="4"/>
+      <c r="AI283" s="4"/>
+      <c r="AJ283" s="4"/>
+      <c r="AK283" s="4"/>
+      <c r="AL283" s="4"/>
+      <c r="AM283" s="4"/>
+    </row>
+    <row r="284" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F284" s="4"/>
+      <c r="G284" s="4"/>
+      <c r="H284" s="4"/>
+      <c r="I284" s="4"/>
+      <c r="J284" s="50"/>
+      <c r="K284" s="50"/>
+      <c r="L284" s="50"/>
+      <c r="M284" s="50"/>
+      <c r="N284" s="50"/>
+      <c r="O284" s="50"/>
+      <c r="P284" s="50"/>
+      <c r="Q284" s="50"/>
+      <c r="R284" s="50"/>
+      <c r="V284" s="4"/>
+      <c r="W284" s="4"/>
+      <c r="X284" s="4"/>
+      <c r="Y284" s="4"/>
+      <c r="Z284" s="4"/>
+      <c r="AA284" s="4"/>
+      <c r="AB284" s="4"/>
+      <c r="AC284" s="4"/>
+      <c r="AD284" s="4"/>
+      <c r="AE284" s="4"/>
+      <c r="AF284" s="4"/>
+      <c r="AG284" s="4"/>
+      <c r="AH284" s="4"/>
+      <c r="AI284" s="4"/>
+      <c r="AJ284" s="4"/>
+      <c r="AK284" s="4"/>
+      <c r="AL284" s="4"/>
+      <c r="AM284" s="4"/>
+    </row>
+    <row r="285" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F285" s="4"/>
+      <c r="G285" s="4"/>
+      <c r="H285" s="4"/>
+      <c r="I285" s="50"/>
+      <c r="J285" s="50"/>
+      <c r="K285" s="50"/>
+      <c r="L285" s="50"/>
+      <c r="M285" s="50"/>
+      <c r="N285" s="50"/>
+      <c r="O285" s="50"/>
+      <c r="P285" s="50"/>
+      <c r="Q285" s="50"/>
+      <c r="R285" s="50"/>
+      <c r="V285" s="4"/>
+      <c r="W285" s="4"/>
+      <c r="X285">
+        <v>13</v>
+      </c>
+      <c r="Y285">
+        <v>14</v>
+      </c>
+      <c r="Z285">
+        <v>15</v>
+      </c>
+      <c r="AA285">
+        <v>16</v>
+      </c>
+      <c r="AB285">
+        <v>17</v>
+      </c>
+      <c r="AC285" s="4"/>
+      <c r="AD285" s="4"/>
+      <c r="AE285" s="4"/>
+      <c r="AF285" s="4"/>
+      <c r="AG285" s="4"/>
+      <c r="AH285" s="4"/>
+      <c r="AI285" s="4"/>
+      <c r="AJ285" s="4"/>
+      <c r="AK285" s="4"/>
+      <c r="AL285" s="4"/>
+      <c r="AM285" s="4"/>
+    </row>
+    <row r="286" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F286" s="4"/>
+      <c r="G286" s="4"/>
+      <c r="H286" s="4"/>
+      <c r="I286" s="4"/>
+      <c r="J286" s="4"/>
+      <c r="K286" s="50"/>
+      <c r="L286" s="50"/>
+      <c r="M286" s="50"/>
+      <c r="N286" s="50"/>
+      <c r="O286" s="50"/>
+      <c r="P286" s="34"/>
+      <c r="Q286" s="42"/>
+      <c r="R286" s="42"/>
+      <c r="V286" s="4"/>
+      <c r="W286" s="4"/>
+      <c r="X286" s="50"/>
+      <c r="Y286" s="50"/>
+      <c r="Z286" s="34"/>
+      <c r="AA286" s="42"/>
+      <c r="AB286" s="42"/>
+      <c r="AC286" s="4"/>
+      <c r="AD286" s="4"/>
+      <c r="AE286" s="4"/>
+      <c r="AF286" s="4"/>
+      <c r="AG286" s="4"/>
+      <c r="AH286" s="4"/>
+      <c r="AI286" s="4"/>
+      <c r="AJ286" s="4"/>
+      <c r="AK286" s="4"/>
+      <c r="AL286" s="4"/>
+      <c r="AM286" s="4"/>
+    </row>
+    <row r="287" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F287" s="4"/>
+      <c r="G287" s="4"/>
+      <c r="H287" s="4"/>
+      <c r="I287" s="50"/>
+      <c r="J287" s="50"/>
+      <c r="K287" s="50"/>
+      <c r="L287" s="50"/>
+      <c r="M287" s="50"/>
+      <c r="N287" s="50"/>
+      <c r="O287" s="41"/>
+      <c r="P287" s="35"/>
+      <c r="Q287" s="41"/>
+      <c r="R287" s="50"/>
+      <c r="V287" s="4"/>
+      <c r="W287" s="4"/>
+      <c r="X287" s="50"/>
+      <c r="Y287" s="41"/>
+      <c r="Z287" s="35"/>
+      <c r="AA287" s="41"/>
+      <c r="AB287" s="50"/>
+      <c r="AC287" s="4"/>
+      <c r="AD287" s="4"/>
+      <c r="AE287" s="4"/>
+      <c r="AF287" s="4"/>
+      <c r="AG287" s="4"/>
+      <c r="AH287" s="4"/>
+      <c r="AI287" s="4"/>
+      <c r="AJ287" s="4"/>
+      <c r="AK287" s="4"/>
+      <c r="AL287" s="4"/>
+      <c r="AM287" s="4"/>
+    </row>
+    <row r="288" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F288" s="4"/>
+      <c r="G288" s="4"/>
+      <c r="H288" s="4"/>
+      <c r="I288" s="50"/>
+      <c r="J288" s="50"/>
+      <c r="K288" s="50"/>
+      <c r="L288" s="50"/>
+      <c r="M288" s="50"/>
+      <c r="N288" s="41"/>
+      <c r="O288" s="41"/>
+      <c r="P288" s="35"/>
+      <c r="Q288" s="50"/>
+      <c r="R288" s="50"/>
+      <c r="V288" s="4"/>
+      <c r="W288" s="4"/>
+      <c r="X288" s="41"/>
+      <c r="Y288" s="41"/>
+      <c r="Z288" s="35"/>
+      <c r="AA288" s="50"/>
+      <c r="AB288" s="50"/>
+      <c r="AC288" s="4"/>
+      <c r="AD288" s="4"/>
+      <c r="AE288" s="4"/>
+      <c r="AF288" s="4"/>
+      <c r="AG288" s="4"/>
+      <c r="AH288" s="4"/>
+      <c r="AI288" s="4"/>
+      <c r="AJ288" s="4"/>
+      <c r="AK288" s="4"/>
+      <c r="AL288" s="4"/>
+      <c r="AM288" s="4"/>
+    </row>
+    <row r="289" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A289" s="4"/>
+      <c r="B289" s="4"/>
+      <c r="C289" s="4"/>
+      <c r="D289" s="4"/>
+      <c r="E289" s="4"/>
+      <c r="F289" s="4"/>
+      <c r="G289" s="4"/>
+      <c r="H289" s="4"/>
+      <c r="I289" s="50"/>
+      <c r="J289" s="4"/>
+      <c r="K289" s="4"/>
+      <c r="L289" s="50"/>
+      <c r="M289" s="50"/>
+      <c r="N289" s="50"/>
+      <c r="O289" s="50"/>
+      <c r="P289" s="26"/>
+      <c r="Q289" s="50"/>
+      <c r="R289" s="50"/>
+      <c r="V289" s="4"/>
+      <c r="W289" s="4"/>
+      <c r="X289" s="50"/>
+      <c r="Y289" s="50"/>
+      <c r="Z289" s="26"/>
+      <c r="AA289" s="50"/>
+      <c r="AB289" s="50"/>
+      <c r="AC289" s="4"/>
+      <c r="AD289" s="4"/>
+      <c r="AE289" s="4"/>
+      <c r="AF289" s="4"/>
+      <c r="AG289" s="4"/>
+      <c r="AH289" s="4"/>
+      <c r="AI289" s="4"/>
+      <c r="AJ289" s="4"/>
+      <c r="AK289" s="4"/>
+      <c r="AL289" s="4"/>
+      <c r="AM289" s="4"/>
+    </row>
+    <row r="290" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A290" s="4"/>
+      <c r="B290" s="4"/>
+      <c r="C290" s="4"/>
+      <c r="D290" s="4"/>
+      <c r="E290" s="4"/>
+      <c r="F290" s="4"/>
+      <c r="G290" s="4"/>
+      <c r="H290" s="4"/>
+      <c r="I290" s="4"/>
+      <c r="J290" s="4"/>
+      <c r="K290" s="50"/>
+      <c r="L290" s="50"/>
+      <c r="M290" s="50"/>
+      <c r="N290" s="50"/>
+      <c r="O290" s="43"/>
+      <c r="P290" s="36"/>
+      <c r="Q290" s="50"/>
+      <c r="R290" s="50"/>
+      <c r="V290" s="4"/>
+      <c r="W290" s="4"/>
+      <c r="X290" s="50"/>
+      <c r="Y290" s="43"/>
+      <c r="Z290" s="36"/>
+      <c r="AA290" s="50"/>
+      <c r="AB290" s="50"/>
+      <c r="AC290" s="4"/>
+      <c r="AD290" s="4"/>
+      <c r="AE290" s="4"/>
+      <c r="AF290" s="4"/>
+      <c r="AG290" s="4"/>
+      <c r="AH290" s="4"/>
+      <c r="AI290" s="4"/>
+      <c r="AJ290" s="4"/>
+      <c r="AK290" s="4"/>
+      <c r="AL290" s="4"/>
+      <c r="AM290" s="4"/>
+    </row>
+    <row r="291" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="4"/>
+      <c r="B291" s="4"/>
+      <c r="C291" s="4"/>
+      <c r="D291" s="4"/>
+      <c r="E291" s="4"/>
+      <c r="F291" s="4"/>
+      <c r="G291" s="4"/>
+      <c r="H291" s="4"/>
+      <c r="I291" s="4"/>
+      <c r="J291" s="50"/>
+      <c r="K291" s="50"/>
+      <c r="L291" s="50"/>
+      <c r="M291" s="50"/>
+      <c r="N291" s="50"/>
+      <c r="O291" s="50"/>
+      <c r="P291" s="37"/>
+      <c r="Q291" s="43"/>
+      <c r="R291" s="50"/>
+      <c r="V291" s="4"/>
+      <c r="W291" s="4"/>
+      <c r="X291" s="50"/>
+      <c r="Y291" s="50"/>
+      <c r="Z291" s="37"/>
+      <c r="AA291" s="43"/>
+      <c r="AB291" s="50"/>
+      <c r="AC291" s="4"/>
+      <c r="AD291" s="4"/>
+      <c r="AE291" s="4"/>
+      <c r="AF291" s="4"/>
+      <c r="AG291" s="4"/>
+      <c r="AH291" s="4"/>
+      <c r="AI291" s="4"/>
+      <c r="AJ291" s="4"/>
+      <c r="AK291" s="4"/>
+      <c r="AL291" s="4"/>
+      <c r="AM291" s="4"/>
+    </row>
+    <row r="292" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="4"/>
+      <c r="B292" s="4"/>
+      <c r="C292" s="4"/>
+      <c r="D292" s="4"/>
+      <c r="E292" s="4"/>
+      <c r="F292" s="4"/>
+      <c r="G292" s="4"/>
+      <c r="H292" s="4"/>
+      <c r="I292" s="50"/>
+      <c r="J292" s="50"/>
+      <c r="K292" s="50"/>
+      <c r="L292" s="50"/>
+      <c r="M292" s="50"/>
+      <c r="N292" s="50"/>
+      <c r="O292" s="50"/>
+      <c r="P292" s="50"/>
+      <c r="Q292" s="50"/>
+      <c r="R292" s="50"/>
+      <c r="V292" s="4"/>
+      <c r="W292" s="4"/>
+      <c r="X292">
+        <v>13</v>
+      </c>
+      <c r="Y292">
+        <v>14</v>
+      </c>
+      <c r="Z292">
+        <v>15</v>
+      </c>
+      <c r="AA292">
+        <v>16</v>
+      </c>
+      <c r="AB292">
+        <v>17</v>
+      </c>
+      <c r="AC292">
+        <v>18</v>
+      </c>
+      <c r="AD292" s="4"/>
+      <c r="AE292" s="4"/>
+      <c r="AF292" s="4"/>
+      <c r="AG292" s="4"/>
+      <c r="AH292" s="4"/>
+      <c r="AI292" s="4"/>
+      <c r="AJ292" s="4"/>
+      <c r="AK292" s="4"/>
+      <c r="AL292" s="4"/>
+      <c r="AM292" s="4"/>
+    </row>
+    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F293" s="4"/>
+      <c r="G293" s="4"/>
+      <c r="H293" s="50"/>
+      <c r="I293" s="50"/>
+      <c r="J293" s="50"/>
+      <c r="K293" s="50"/>
+      <c r="L293" s="50"/>
+      <c r="M293" s="50"/>
+      <c r="N293" s="50"/>
+      <c r="O293" s="50"/>
+      <c r="P293" s="46"/>
+      <c r="Q293" s="38"/>
+      <c r="R293" s="41"/>
+      <c r="S293" s="41"/>
+      <c r="X293" s="50"/>
+      <c r="Y293" s="50"/>
+      <c r="Z293" s="46"/>
+      <c r="AA293" s="38"/>
+      <c r="AB293" s="41"/>
+      <c r="AC293" s="41"/>
+    </row>
+    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F294" s="4"/>
+      <c r="G294" s="4"/>
+      <c r="H294" s="4"/>
+      <c r="I294" s="4"/>
+      <c r="J294" s="50"/>
+      <c r="K294" s="50"/>
+      <c r="L294" s="50"/>
+      <c r="M294" s="50"/>
+      <c r="N294" s="50"/>
+      <c r="O294" s="50"/>
+      <c r="P294" s="44"/>
+      <c r="Q294" s="39"/>
+      <c r="R294" s="42"/>
+      <c r="X294" s="50"/>
+      <c r="Y294" s="50"/>
+      <c r="Z294" s="44"/>
+      <c r="AA294" s="39"/>
+      <c r="AB294" s="42"/>
+    </row>
+    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F295" s="4"/>
+      <c r="G295" s="4"/>
+      <c r="H295" s="4"/>
+      <c r="I295" s="4"/>
+      <c r="J295" s="4"/>
+      <c r="K295" s="50"/>
+      <c r="L295" s="50"/>
+      <c r="M295" s="50"/>
+      <c r="N295" s="50"/>
+      <c r="O295" s="41"/>
+      <c r="P295" s="45"/>
+      <c r="Q295" s="40"/>
+      <c r="R295" s="50"/>
+      <c r="X295" s="50"/>
+      <c r="Y295" s="41"/>
+      <c r="Z295" s="45"/>
+      <c r="AA295" s="40"/>
+      <c r="AB295" s="50"/>
+    </row>
+    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F296" s="4"/>
+      <c r="G296" s="4"/>
+      <c r="H296" s="4"/>
+      <c r="I296" s="50"/>
+      <c r="J296" s="4"/>
+      <c r="K296" s="50"/>
+      <c r="L296" s="50"/>
+      <c r="M296" s="50"/>
+      <c r="N296" s="41"/>
+      <c r="O296" s="41"/>
+      <c r="P296" s="45"/>
+      <c r="Q296" s="48"/>
+      <c r="R296" s="50"/>
+      <c r="X296" s="41"/>
+      <c r="Y296" s="41"/>
+      <c r="Z296" s="45"/>
+      <c r="AA296" s="48"/>
+      <c r="AB296" s="50"/>
+    </row>
+    <row r="297" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F297" s="4"/>
+      <c r="G297" s="4"/>
+      <c r="H297" s="4"/>
+      <c r="I297" s="50"/>
+      <c r="J297" s="50"/>
+      <c r="K297" s="50"/>
+      <c r="L297" s="50"/>
+      <c r="M297" s="50"/>
+      <c r="N297" s="50"/>
+      <c r="O297" s="50"/>
+      <c r="P297" s="19"/>
+      <c r="Q297" s="21"/>
+      <c r="R297" s="50"/>
+      <c r="X297" s="50"/>
+      <c r="Y297" s="50"/>
+      <c r="Z297" s="19"/>
+      <c r="AA297" s="21"/>
+      <c r="AB297" s="50"/>
+    </row>
+    <row r="298" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F298" s="4"/>
+      <c r="G298" s="4"/>
+      <c r="H298" s="4"/>
+      <c r="I298" s="50"/>
+      <c r="J298" s="50"/>
+      <c r="K298" s="50"/>
+      <c r="L298" s="50"/>
+      <c r="M298" s="50"/>
+      <c r="N298" s="50"/>
+      <c r="O298" s="50"/>
+      <c r="P298" s="50"/>
+      <c r="Q298" s="50"/>
+      <c r="R298" s="50"/>
+    </row>
+    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F299" s="4"/>
+      <c r="G299" s="4"/>
+      <c r="H299" s="4"/>
+      <c r="I299" s="4"/>
+      <c r="J299" s="50"/>
+      <c r="K299" s="50"/>
+      <c r="L299" s="50"/>
+      <c r="M299" s="50"/>
+      <c r="N299" s="50"/>
+      <c r="O299" s="50"/>
+      <c r="P299" s="46"/>
+      <c r="Q299" s="52"/>
+      <c r="R299" s="38"/>
+      <c r="S299" s="41"/>
+      <c r="T299" s="41"/>
+    </row>
+    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F300" s="4"/>
+      <c r="G300" s="4"/>
+      <c r="H300" s="4"/>
+      <c r="I300" s="4"/>
+      <c r="J300" s="4"/>
+      <c r="K300" s="50"/>
+      <c r="L300" s="50"/>
+      <c r="M300" s="50"/>
+      <c r="N300" s="50"/>
+      <c r="O300" s="50"/>
+      <c r="P300" s="47"/>
+      <c r="Q300" s="41"/>
+      <c r="R300" s="40"/>
+      <c r="S300" s="41"/>
+    </row>
+    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F301" s="4"/>
+      <c r="G301" s="4"/>
+      <c r="H301" s="4"/>
+      <c r="I301" s="50"/>
+      <c r="J301" s="4"/>
+      <c r="K301" s="4"/>
+      <c r="L301" s="50"/>
+      <c r="M301" s="50"/>
+      <c r="N301" s="50"/>
+      <c r="O301" s="50"/>
+      <c r="P301" s="44"/>
+      <c r="Q301" s="42"/>
+      <c r="R301" s="39"/>
+    </row>
+    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F302" s="4"/>
+      <c r="G302" s="4"/>
+      <c r="H302" s="4"/>
+      <c r="I302" s="50"/>
+      <c r="J302" s="50"/>
+      <c r="K302" s="50"/>
+      <c r="L302" s="50"/>
+      <c r="M302" s="50"/>
+      <c r="N302" s="50"/>
+      <c r="O302" s="41"/>
+      <c r="P302" s="45"/>
+      <c r="Q302" s="41"/>
+      <c r="R302" s="48"/>
+    </row>
+    <row r="303" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F303" s="4"/>
+      <c r="G303" s="4"/>
+      <c r="H303" s="4"/>
+      <c r="I303" s="50"/>
+      <c r="J303" s="50"/>
+      <c r="K303" s="50"/>
+      <c r="L303" s="50"/>
+      <c r="M303" s="50"/>
+      <c r="N303" s="41"/>
+      <c r="O303" s="41"/>
+      <c r="P303" s="53"/>
+      <c r="Q303" s="51"/>
+      <c r="R303" s="49"/>
+    </row>
+    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="F304" s="4"/>
+      <c r="G304" s="4"/>
+      <c r="H304" s="4"/>
+      <c r="I304" s="50"/>
+      <c r="J304" s="50"/>
+      <c r="K304" s="50"/>
+      <c r="L304" s="50"/>
+      <c r="M304" s="50"/>
+      <c r="N304" s="50"/>
+      <c r="O304" s="50"/>
+      <c r="P304" s="50"/>
+      <c r="Q304" s="50"/>
+      <c r="R304" s="50"/>
+    </row>
+    <row r="305" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F305" s="4"/>
+      <c r="G305" s="4"/>
+      <c r="H305" s="4"/>
+      <c r="I305" s="50"/>
+      <c r="J305" s="50"/>
+      <c r="K305" s="50"/>
+      <c r="L305" s="50"/>
+      <c r="M305" s="50"/>
+      <c r="Z305">
+        <v>15</v>
+      </c>
+      <c r="AA305">
+        <v>16</v>
+      </c>
+      <c r="AB305">
+        <v>17</v>
+      </c>
+      <c r="AC305" s="50"/>
+      <c r="AD305" s="50"/>
+      <c r="AE305" s="50"/>
+      <c r="AF305" s="50"/>
+      <c r="AG305" s="50"/>
+    </row>
+    <row r="306" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F306" s="4"/>
+      <c r="G306" s="4"/>
+      <c r="H306" s="4"/>
+      <c r="I306" s="4"/>
+      <c r="J306" s="50"/>
+      <c r="K306" s="50"/>
+      <c r="L306" s="50"/>
+      <c r="M306" s="50"/>
+      <c r="P306" s="3"/>
+      <c r="Z306" s="3"/>
+      <c r="AC306" s="50"/>
+      <c r="AD306" s="50"/>
+      <c r="AE306" s="50"/>
+      <c r="AF306" s="50"/>
+      <c r="AG306" s="50"/>
+    </row>
+    <row r="307" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F307" s="4"/>
+      <c r="G307" s="4"/>
+      <c r="H307" s="4"/>
+      <c r="I307" s="4"/>
+      <c r="J307" s="4"/>
+      <c r="K307" s="50"/>
+      <c r="L307" s="50"/>
+      <c r="M307" s="50"/>
+      <c r="P307" s="33"/>
+      <c r="Q307" s="33"/>
+      <c r="R307" s="33"/>
+      <c r="Z307" s="33"/>
+      <c r="AA307" s="33"/>
+      <c r="AB307" s="33"/>
+      <c r="AC307" s="50"/>
+      <c r="AD307" s="50"/>
+      <c r="AE307" s="50"/>
+      <c r="AF307" s="50"/>
+      <c r="AG307" s="50"/>
+    </row>
+    <row r="308" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F308" s="4"/>
+      <c r="G308" s="4"/>
+      <c r="H308" s="4"/>
+      <c r="I308" s="50"/>
+      <c r="J308" s="4"/>
+      <c r="K308" s="4"/>
+      <c r="L308" s="50"/>
+      <c r="M308" s="50"/>
+      <c r="Q308" s="3"/>
+      <c r="AA308" s="3"/>
+      <c r="AC308" s="50"/>
+      <c r="AD308" s="50"/>
+      <c r="AE308" s="50"/>
+      <c r="AF308" s="50"/>
+      <c r="AG308" s="50"/>
+    </row>
+    <row r="309" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F309" s="4"/>
+      <c r="G309" s="4"/>
+      <c r="H309" s="4"/>
+      <c r="I309" s="50"/>
+      <c r="J309" s="50"/>
+      <c r="K309" s="50"/>
+      <c r="L309" s="50"/>
+      <c r="M309" s="50"/>
+      <c r="R309" s="3"/>
+      <c r="AB309" s="3"/>
+      <c r="AC309" s="50"/>
+      <c r="AD309" s="50"/>
+      <c r="AE309" s="50"/>
+      <c r="AF309" s="50"/>
+      <c r="AG309" s="50"/>
+    </row>
+    <row r="310" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F310" s="4"/>
+      <c r="G310" s="4"/>
+      <c r="H310" s="4"/>
+      <c r="I310" s="4"/>
+      <c r="J310" s="50"/>
+      <c r="K310" s="50"/>
+      <c r="L310" s="50"/>
+      <c r="M310" s="50"/>
+      <c r="AA310" s="50"/>
+      <c r="AB310" s="50"/>
+      <c r="AC310" s="50"/>
+      <c r="AD310" s="50"/>
+      <c r="AE310" s="50"/>
+      <c r="AF310" s="50"/>
+      <c r="AG310" s="50"/>
+    </row>
+    <row r="311" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F311" s="4"/>
+      <c r="G311" s="4"/>
+      <c r="H311" s="4"/>
+      <c r="I311" s="4"/>
+      <c r="J311" s="4"/>
+      <c r="K311" s="50"/>
+      <c r="L311" s="50"/>
+      <c r="M311" s="50"/>
+      <c r="Z311">
+        <v>14</v>
+      </c>
+      <c r="AA311">
+        <v>15</v>
+      </c>
+      <c r="AB311">
+        <v>16</v>
+      </c>
+      <c r="AC311">
+        <v>17</v>
+      </c>
+      <c r="AD311">
+        <v>18</v>
+      </c>
+      <c r="AE311" s="50"/>
+      <c r="AF311" s="50"/>
+      <c r="AG311" s="50"/>
+    </row>
+    <row r="312" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="F312" s="4"/>
+      <c r="G312" s="4"/>
+      <c r="H312" s="4"/>
+      <c r="I312" s="50"/>
+      <c r="J312" s="4"/>
+      <c r="K312" s="4"/>
+      <c r="L312" s="50"/>
+      <c r="M312" s="50"/>
+      <c r="O312" s="2"/>
+      <c r="P312" s="2"/>
+      <c r="Z312" s="2"/>
+      <c r="AA312" s="2"/>
+      <c r="AE312" s="50"/>
+      <c r="AF312" s="50"/>
+      <c r="AG312" s="50"/>
+    </row>
+    <row r="313" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="P313" s="33"/>
+      <c r="Q313" s="33"/>
+      <c r="R313" s="33"/>
+      <c r="AA313" s="33"/>
+      <c r="AB313" s="33"/>
+      <c r="AC313" s="33"/>
+      <c r="AE313" s="50"/>
+      <c r="AF313" s="50"/>
+    </row>
+    <row r="314" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="P314" s="2"/>
+      <c r="Q314" s="2"/>
+      <c r="AA314" s="2"/>
+      <c r="AB314" s="2"/>
+      <c r="AE314" s="4"/>
+      <c r="AF314" s="4"/>
+      <c r="AG314" s="4"/>
+    </row>
+    <row r="315" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="Q315" s="2"/>
+      <c r="R315" s="2"/>
+      <c r="AB315" s="2"/>
+      <c r="AC315" s="2"/>
+    </row>
+    <row r="316" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="R316" s="2"/>
+      <c r="S316" s="2"/>
+      <c r="AC316" s="2"/>
+      <c r="AD316" s="2"/>
+    </row>
+    <row r="318" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="N318" s="3"/>
+      <c r="O318" s="3"/>
+      <c r="P318" s="3"/>
+      <c r="Q318" s="3"/>
+      <c r="R318" s="3"/>
+      <c r="S318" s="4"/>
+    </row>
+    <row r="319" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="O319" s="3"/>
+      <c r="P319" s="3"/>
+      <c r="Q319" s="3"/>
+      <c r="R319" s="3"/>
+      <c r="S319" s="3"/>
+      <c r="T319" s="4"/>
+    </row>
+    <row r="320" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="P320" s="3"/>
+      <c r="Q320" s="3"/>
+      <c r="R320" s="3"/>
+      <c r="S320" s="3"/>
+      <c r="T320" s="3"/>
+      <c r="U320" s="3"/>
+      <c r="V320" s="4"/>
+    </row>
+    <row r="321" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="Q321" s="3"/>
+      <c r="R321" s="3"/>
+      <c r="S321" s="3"/>
+      <c r="T321" s="3"/>
+      <c r="U321" s="3"/>
+      <c r="V321" s="3"/>
+      <c r="W321" s="4"/>
+    </row>
+    <row r="322" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="R322" s="3"/>
+      <c r="S322" s="3"/>
+      <c r="T322" s="3"/>
+      <c r="U322" s="3"/>
+      <c r="V322" s="3"/>
+      <c r="W322" s="3"/>
+      <c r="X322" s="4"/>
+    </row>
+    <row r="323" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="S323" s="3"/>
+      <c r="T323" s="3"/>
+      <c r="U323" s="3"/>
+      <c r="V323" s="3"/>
+      <c r="W323" s="3"/>
+      <c r="X323" s="3"/>
+      <c r="Y323" s="4"/>
+    </row>
+    <row r="324" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="T324" s="3"/>
+      <c r="U324" s="3"/>
+      <c r="V324" s="3"/>
+      <c r="W324" s="3"/>
+      <c r="X324" s="3"/>
+      <c r="Y324" s="3"/>
+      <c r="Z324" s="4"/>
+    </row>
+    <row r="325" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="V325" s="3"/>
+      <c r="W325" s="3"/>
+      <c r="X325" s="3"/>
+      <c r="Y325" s="3"/>
+      <c r="Z325" s="3"/>
+      <c r="AA325" s="4"/>
+    </row>
+    <row r="326" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="W326" s="3"/>
+      <c r="X326" s="3"/>
+      <c r="Y326" s="3"/>
+      <c r="Z326" s="3"/>
+      <c r="AA326" s="3"/>
+    </row>
+    <row r="328" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="P328" s="1"/>
+      <c r="Q328" s="1"/>
+      <c r="R328" s="1"/>
+      <c r="S328" s="1"/>
+      <c r="T328" s="1"/>
+      <c r="U328" s="1"/>
+      <c r="V328" s="1"/>
+      <c r="W328" s="1"/>
+      <c r="X328" s="1"/>
+      <c r="Y328" s="1"/>
+    </row>
+    <row r="329" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="Q329" s="1"/>
+      <c r="R329" s="1"/>
+      <c r="S329" s="1"/>
+      <c r="T329" s="1"/>
+      <c r="U329" s="1"/>
+      <c r="V329" s="1"/>
+      <c r="W329" s="1"/>
+      <c r="X329" s="1"/>
+      <c r="Y329" s="1"/>
+      <c r="Z329" s="1"/>
+    </row>
+    <row r="330" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="R330" s="1"/>
+      <c r="S330" s="1"/>
+      <c r="T330" s="1"/>
+      <c r="U330" s="1"/>
+      <c r="V330" s="1"/>
+      <c r="W330" s="1"/>
+      <c r="X330" s="1"/>
+      <c r="Y330" s="1"/>
+      <c r="Z330" s="1"/>
+      <c r="AA330" s="1"/>
+    </row>
+    <row r="331" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="R331" s="2"/>
+      <c r="S331" s="2"/>
+      <c r="T331" s="2"/>
+      <c r="U331" s="2"/>
+      <c r="V331" s="2"/>
+      <c r="W331" s="2"/>
+      <c r="X331" s="2"/>
+      <c r="Y331" s="2"/>
+      <c r="Z331" s="2"/>
+    </row>
+    <row r="332" spans="16:27" x14ac:dyDescent="0.25">
+      <c r="U332" s="4"/>
+    </row>
+    <row r="339" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="AB339" s="4"/>
+    </row>
+    <row r="346" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K346" s="4"/>
+      <c r="L346" s="4"/>
+      <c r="M346" s="4"/>
+      <c r="N346" s="4"/>
+      <c r="O346" s="4"/>
+      <c r="P346" s="4"/>
+      <c r="Q346" s="4"/>
+    </row>
+    <row r="347" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K347" s="4"/>
+      <c r="L347" s="4"/>
+      <c r="M347" s="4"/>
+      <c r="N347" s="4"/>
+      <c r="O347" s="4"/>
+      <c r="P347" s="4"/>
+      <c r="Q347" s="4"/>
+      <c r="S347" s="3"/>
+    </row>
+    <row r="348" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K348" s="4"/>
+      <c r="L348" s="4"/>
+      <c r="M348" s="4"/>
+      <c r="N348" s="2"/>
+      <c r="O348" s="2"/>
+      <c r="P348" s="2"/>
+      <c r="Q348" s="2"/>
+      <c r="R348" s="2"/>
+    </row>
+    <row r="349" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K349" s="4"/>
+      <c r="L349" s="4"/>
+      <c r="M349" s="4"/>
+      <c r="N349" s="4"/>
+      <c r="O349" s="2"/>
+      <c r="P349" s="2"/>
+      <c r="Q349" s="2"/>
+      <c r="R349" s="2"/>
+      <c r="S349" s="2"/>
+    </row>
+    <row r="350" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K350" s="4"/>
+      <c r="L350" s="4"/>
+      <c r="M350" s="4"/>
+      <c r="N350" s="4"/>
+      <c r="O350" s="4"/>
+      <c r="P350" s="2"/>
+      <c r="Q350" s="2"/>
+      <c r="R350" s="2"/>
+      <c r="S350" s="2"/>
+      <c r="T350" s="2"/>
+    </row>
+    <row r="351" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K351" s="4"/>
+      <c r="L351" s="4"/>
+      <c r="M351" s="4"/>
+      <c r="N351" s="4"/>
+      <c r="O351" s="4"/>
+      <c r="P351" s="4"/>
+      <c r="Q351" s="2"/>
+      <c r="R351" s="2"/>
+      <c r="S351" s="2"/>
+      <c r="T351" s="2"/>
+      <c r="U351" s="2"/>
+    </row>
+    <row r="352" spans="11:28" x14ac:dyDescent="0.25">
+      <c r="K352" s="4"/>
+      <c r="L352" s="4"/>
+      <c r="M352" s="4"/>
+      <c r="N352" s="4"/>
+      <c r="O352" s="4"/>
+      <c r="P352" s="4"/>
+      <c r="Q352" s="4"/>
+      <c r="R352" s="2"/>
+      <c r="S352" s="2"/>
+      <c r="T352" s="2"/>
+      <c r="U352" s="2"/>
+      <c r="V352" s="2"/>
+    </row>
+    <row r="353" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="S353" s="2"/>
+      <c r="T353" s="2"/>
+      <c r="U353" s="2"/>
+      <c r="V353" s="2"/>
+      <c r="W353" s="2"/>
+    </row>
+    <row r="354" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="Q354" s="1"/>
+      <c r="R354" s="1"/>
+      <c r="S354" s="1"/>
+    </row>
+    <row r="355" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="R355" s="1"/>
+      <c r="S355" s="1"/>
+      <c r="T355" s="1"/>
+    </row>
+    <row r="356" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="S356" s="1"/>
+      <c r="T356" s="1"/>
+      <c r="U356" s="1"/>
+    </row>
+    <row r="357" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O357" s="28"/>
+      <c r="P357" s="28"/>
+      <c r="Q357" s="28"/>
+      <c r="R357" s="28"/>
+      <c r="S357" s="28"/>
+      <c r="T357" s="1"/>
+      <c r="U357" s="1"/>
+    </row>
+    <row r="358" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="P358" s="28"/>
+      <c r="Q358" s="28"/>
+      <c r="R358" s="28"/>
+      <c r="S358" s="28"/>
+      <c r="T358" s="28"/>
+    </row>
+    <row r="359" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="Q359" s="28"/>
+      <c r="R359" s="28"/>
+      <c r="S359" s="28"/>
+      <c r="T359" s="28"/>
+      <c r="U359" s="28"/>
+    </row>
+    <row r="360" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="R360" s="28"/>
+      <c r="S360" s="28"/>
+      <c r="T360" s="28"/>
+      <c r="U360" s="28"/>
+      <c r="V360" s="28"/>
+    </row>
+    <row r="361" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="S361" s="28"/>
+      <c r="T361" s="28"/>
+      <c r="U361" s="28"/>
+      <c r="V361" s="28"/>
+      <c r="W361" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>